<commit_message>
update config file for deepstream
</commit_message>
<xml_diff>
--- a/deepstream/配置文件属性.xlsx
+++ b/deepstream/配置文件属性.xlsx
@@ -486,9 +486,6 @@
   </si>
   <si>
     <t>interval=2</t>
-  </si>
-  <si>
-    <t>bbox-border-color</t>
   </si>
   <si>
     <r>
@@ -1589,6 +1586,10 @@
   </si>
   <si>
     <t>Type of CUDA memory element is to allocate for output buffers.0 (cuda-pinned-mem): host/pinned memory allocated with cudaMallocHost().1 (cuda-device-mem): Device memory allocated with cudaMalloc().2 (cuda-unified-mem): Unified memory allocated with cudaMallocManaged().</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>bbox-border-color</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -2165,7 +2166,7 @@
   <sheetData>
     <row r="2" spans="2:3" ht="36.950000000000003" customHeight="1" thickBot="1">
       <c r="B2" s="15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C2" s="16"/>
     </row>
@@ -2246,7 +2247,7 @@
         <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15" thickBot="1">
@@ -2271,8 +2272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2287,7 +2288,7 @@
   <sheetData>
     <row r="2" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A2" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -2496,7 +2497,7 @@
         <v>58</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>59</v>
@@ -2513,7 +2514,7 @@
         <v>61</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>62</v>
@@ -2574,7 +2575,7 @@
         <v>66</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>67</v>
@@ -2597,7 +2598,7 @@
         <v>37</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>31</v>
@@ -2614,7 +2615,7 @@
         <v>59</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>31</v>
@@ -2631,7 +2632,7 @@
         <v>30</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>31</v>
@@ -2812,7 +2813,7 @@
         <v>105</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>106</v>
@@ -2829,7 +2830,7 @@
         <v>61</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>108</v>
@@ -2941,7 +2942,7 @@
         <v>52</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>34</v>
@@ -2972,16 +2973,16 @@
     </row>
     <row r="47" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A47" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>31</v>
@@ -2992,7 +2993,7 @@
         <v>61</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>124</v>
@@ -3053,10 +3054,10 @@
         <v>129</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>130</v>
@@ -3073,7 +3074,7 @@
         <v>132</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>80</v>
@@ -3104,10 +3105,10 @@
         <v>61</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>125</v>
@@ -3141,7 +3142,7 @@
         <v>141</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>142</v>
@@ -3158,7 +3159,7 @@
         <v>144</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>145</v>
@@ -3169,16 +3170,16 @@
     </row>
     <row r="60" spans="1:5" ht="60.75" customHeight="1" thickBot="1">
       <c r="A60" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>128</v>
@@ -3186,50 +3187,50 @@
     </row>
     <row r="61" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A61" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="D61" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="52.5" customHeight="1" thickBot="1">
       <c r="A62" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="D62" s="1" t="s">
+      <c r="E62" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A63" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>128</v>
@@ -3238,7 +3239,7 @@
     <row r="64" spans="1:5" ht="20.100000000000001" customHeight="1"/>
     <row r="65" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A65" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
@@ -3267,50 +3268,50 @@
         <v>46</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A68" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="E68" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A69" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="E69" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -3318,10 +3319,10 @@
         <v>58</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>80</v>
@@ -3332,59 +3333,59 @@
     </row>
     <row r="71" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A71" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A72" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A73" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="C73" s="1" t="s">
+      <c r="E73" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="20.100000000000001" customHeight="1"/>
     <row r="75" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A75" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B75" s="17"/>
       <c r="C75" s="17"/>
@@ -3413,16 +3414,16 @@
         <v>46</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -3430,10 +3431,10 @@
         <v>58</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>80</v>
@@ -3444,172 +3445,172 @@
     </row>
     <row r="79" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A79" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="E79" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A80" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>178</v>
-      </c>
       <c r="E80" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="55.5" customHeight="1" thickBot="1">
       <c r="A81" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="E81" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="55.5" customHeight="1" thickBot="1">
       <c r="A82" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="E82" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A83" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="C83" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="E83" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A84" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="C84" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C84" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>188</v>
-      </c>
       <c r="E84" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A85" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="C85" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="E85" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="36.75" customHeight="1" thickBot="1">
       <c r="A86" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A87" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="C87" s="1" t="s">
+      <c r="E87" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="58.5" customHeight="1" thickBot="1">
       <c r="A88" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="C88" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D88" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="E88" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="79.5" customHeight="1" thickBot="1">
@@ -3617,10 +3618,10 @@
         <v>61</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>125</v>
@@ -3631,25 +3632,25 @@
     </row>
     <row r="90" spans="1:5" ht="33.75" customHeight="1" thickBot="1">
       <c r="A90" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="C90" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D90" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C90" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>202</v>
-      </c>
       <c r="E90" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="20.100000000000001" customHeight="1"/>
     <row r="92" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A92" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B92" s="17"/>
       <c r="C92" s="17"/>
@@ -3678,16 +3679,16 @@
         <v>46</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="64.5" customHeight="1" thickBot="1">
@@ -3695,152 +3696,152 @@
         <v>66</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="24.75" customHeight="1" thickBot="1">
       <c r="A96" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B96" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="E96" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="48.75" customHeight="1" thickBot="1">
       <c r="A97" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="C97" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D97" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="E97" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="46.5" customHeight="1" thickBot="1">
       <c r="A98" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="E98" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="19.5" customHeight="1" thickBot="1">
       <c r="A99" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B99" s="2" t="s">
-        <v>323</v>
-      </c>
       <c r="C99" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="33.75" customHeight="1" thickBot="1">
       <c r="A100" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D100" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>213</v>
-      </c>
       <c r="E100" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="39.75" customHeight="1" thickBot="1">
       <c r="A101" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D101" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B101" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>215</v>
-      </c>
       <c r="E101" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A102" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B102" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="E102" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A103" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="82.5" customHeight="1" thickBot="1">
@@ -3848,64 +3849,64 @@
         <v>61</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>125</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="42.75" customHeight="1" thickBot="1">
       <c r="A105" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D105" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B105" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>221</v>
-      </c>
       <c r="E105" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="33.75" customHeight="1" thickBot="1">
       <c r="A106" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="C106" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>224</v>
-      </c>
       <c r="E106" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="41.25" customHeight="1" thickBot="1">
       <c r="A107" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="C107" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D107" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>227</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>60</v>
@@ -3916,16 +3917,16 @@
         <v>52</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>114</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -3933,64 +3934,64 @@
         <v>55</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A110" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="C110" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D110" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>231</v>
-      </c>
       <c r="E110" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A111" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="C111" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D111" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C111" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="E111" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A112" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="C112" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>104</v>
@@ -3998,176 +3999,176 @@
     </row>
     <row r="113" spans="1:5" ht="37.5" customHeight="1" thickBot="1">
       <c r="A113" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="C113" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D113" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C113" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>240</v>
-      </c>
       <c r="E113" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="35.25" customHeight="1" thickBot="1">
       <c r="A114" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>242</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="32.25" customHeight="1" thickBot="1">
       <c r="A115" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>245</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A116" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A117" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>250</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="67.5" customHeight="1" thickBot="1">
       <c r="A118" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B118" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="C118" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>254</v>
-      </c>
       <c r="E118" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="40.5" customHeight="1" thickBot="1">
       <c r="A119" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>256</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="75.75" customHeight="1" thickBot="1">
       <c r="A120" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>259</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="52.5" customHeight="1" thickBot="1">
       <c r="A121" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B121" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="C121" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D121" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C121" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>263</v>
-      </c>
       <c r="E121" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="49.5" customHeight="1" thickBot="1">
       <c r="A122" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B122" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="C122" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D122" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="E122" s="1"/>
     </row>
     <row r="123" spans="1:5" ht="20.100000000000001" customHeight="1"/>
     <row r="124" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A124" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B124" s="18"/>
       <c r="C124" s="18"/>
@@ -4193,19 +4194,19 @@
     </row>
     <row r="126" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A126" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B126" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="C126" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="E126" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -4248,7 +4249,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A1" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -4276,284 +4277,284 @@
         <v>115</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="B5" t="s">
+        <v>349</v>
+      </c>
+      <c r="C5" t="s">
+        <v>342</v>
+      </c>
+      <c r="D5" t="s">
         <v>347</v>
-      </c>
-      <c r="B5" t="s">
-        <v>350</v>
-      </c>
-      <c r="C5" t="s">
-        <v>343</v>
-      </c>
-      <c r="D5" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="B6" t="s">
+        <v>351</v>
+      </c>
+      <c r="C6" t="s">
+        <v>350</v>
+      </c>
+      <c r="D6" t="s">
         <v>353</v>
-      </c>
-      <c r="B6" t="s">
-        <v>352</v>
-      </c>
-      <c r="C6" t="s">
-        <v>351</v>
-      </c>
-      <c r="D6" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="B7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C7" t="s">
+        <v>342</v>
+      </c>
+      <c r="D7" t="s">
         <v>356</v>
-      </c>
-      <c r="B7" t="s">
-        <v>355</v>
-      </c>
-      <c r="C7" t="s">
-        <v>343</v>
-      </c>
-      <c r="D7" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B8" t="s">
+        <v>357</v>
+      </c>
+      <c r="C8" t="s">
+        <v>342</v>
+      </c>
+      <c r="D8" t="s">
         <v>358</v>
-      </c>
-      <c r="C8" t="s">
-        <v>343</v>
-      </c>
-      <c r="D8" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="B9" t="s">
+        <v>363</v>
+      </c>
+      <c r="C9" t="s">
+        <v>359</v>
+      </c>
+      <c r="D9" t="s">
         <v>361</v>
-      </c>
-      <c r="B9" t="s">
-        <v>364</v>
-      </c>
-      <c r="C9" t="s">
-        <v>360</v>
-      </c>
-      <c r="D9" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B10" t="s">
+        <v>364</v>
+      </c>
+      <c r="C10" t="s">
         <v>365</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" s="13" t="s">
         <v>366</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="B11" t="s">
         <v>368</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>369</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="13" t="s">
         <v>370</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="B13" t="s">
+        <v>373</v>
+      </c>
+      <c r="C13" t="s">
         <v>372</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>374</v>
-      </c>
-      <c r="C13" t="s">
-        <v>373</v>
-      </c>
-      <c r="D13" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="D14" t="s">
         <v>376</v>
-      </c>
-      <c r="D14" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="B16" t="s">
+        <v>379</v>
+      </c>
+      <c r="C16" t="s">
+        <v>378</v>
+      </c>
+      <c r="D16" t="s">
         <v>381</v>
-      </c>
-      <c r="B16" t="s">
-        <v>380</v>
-      </c>
-      <c r="C16" t="s">
-        <v>379</v>
-      </c>
-      <c r="D16" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="B17" t="s">
         <v>383</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>384</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>385</v>
-      </c>
-      <c r="D17" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="B20" t="s">
+        <v>400</v>
+      </c>
+      <c r="C20" t="s">
+        <v>397</v>
+      </c>
+      <c r="D20" t="s">
         <v>399</v>
-      </c>
-      <c r="B20" t="s">
-        <v>401</v>
-      </c>
-      <c r="C20" t="s">
-        <v>398</v>
-      </c>
-      <c r="D20" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B21" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C21" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B22" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B23" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="8" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B27" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="84" customHeight="1">
       <c r="A28" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="C28" t="s">
         <v>390</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>404</v>
-      </c>
-      <c r="C28" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="116.25" customHeight="1">
       <c r="A29" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="B29" s="14" t="s">
         <v>402</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="20.100000000000001" customHeight="1">
@@ -4561,7 +4562,7 @@
     </row>
     <row r="31" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A31" s="18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
@@ -4583,7 +4584,7 @@
     </row>
     <row r="33" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A33" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
@@ -4593,10 +4594,10 @@
     </row>
     <row r="34" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>